<commit_message>
Robô Concluído e Funcionando, conforme as aulas do Prof.
</commit_message>
<xml_diff>
--- a/Projeto_Final/Data/Config.xlsx
+++ b/Projeto_Final/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Poncetech\UiPath\JornadaRPA\Projeto_Final\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FA11E1-BA9E-4B85-B72D-53B39B0C1D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1275" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -123,12 +123,30 @@
   <si>
     <t>OrchestratorAssetFolder</t>
   </si>
+  <si>
+    <t>DesafiosRPAURL</t>
+  </si>
+  <si>
+    <t>https://desafiosrpa.com.br/login.html</t>
+  </si>
+  <si>
+    <t>Endereço URL do Sistema</t>
+  </si>
+  <si>
+    <t>DesafiosRPACredential</t>
+  </si>
+  <si>
+    <t>DesafiosRPA</t>
+  </si>
+  <si>
+    <t>Nome do Asset no Orchestrator</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -152,6 +170,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -170,10 +194,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -183,8 +208,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -201,7 +228,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -499,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -569,9 +596,29 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1563,8 +1610,11 @@
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{1DB9C938-296E-446B-9105-2F6621BBE065}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1572,7 +1622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1621,7 +1673,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>26</v>
@@ -2682,7 +2734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>